<commit_message>
Added test cases - functions - test data - for CatalogOfContent Section.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Variable</t>
   </si>
@@ -44,12 +44,12 @@
     <t>MicrosoftInternetExplorer</t>
   </si>
   <si>
+    <t>#/login</t>
+  </si>
+  <si>
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>#/login</t>
-  </si>
-  <si>
     <t>URL_content</t>
   </si>
   <si>
@@ -125,79 +125,10 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Automation_Dashboard_Delete_ForVerification</t>
+    <t>Automation_Dashboard_CatalogOfContent</t>
   </si>
   <si>
     <t>New Dashboard</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_NeverMind</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_ConfirmationMessage</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_Arabic</t>
-  </si>
-  <si>
-    <t>لوحة التحكم الآليلوحة التحكم الآلي</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_SpecialCharecters</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_SpecialCharecters!@#[]</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_SchemaNotLoaded</t>
-  </si>
-  <si>
-    <t>New Dashboard - With schema not loaded</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_NoInsights</t>
-  </si>
-  <si>
-    <t>New Dashboard - No Insights</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_SharedEdit</t>
-  </si>
-  <si>
-    <t>New Dashboard Shared edit</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_SharedShare</t>
-  </si>
-  <si>
-    <t>New Dashboard Shared share</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_SharedView</t>
-  </si>
-  <si>
-    <t>New Dashboard Shared view</t>
-  </si>
-  <si>
-    <t>Automation_Folder_Delete</t>
-  </si>
-  <si>
-    <t>New Folder</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_UnderFolder</t>
-  </si>
-  <si>
-    <t>New Dashboard Created under folder [Automation_Folder_Delete]</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_LongName</t>
-  </si>
-  <si>
-    <t>Automation_Dashboard_Delete_LongName . Automation_Dashboard_Delete_LongNameAutomation_Dashboard_Delete_LongName</t>
   </si>
 </sst>
 </file>
@@ -441,7 +372,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -771,15 +702,9 @@
       <c r="O17" s="7"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -794,15 +719,9 @@
       <c r="O18" s="6"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -817,15 +736,9 @@
       <c r="O19" s="7"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -840,15 +753,9 @@
       <c r="O20" s="7"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -863,15 +770,9 @@
       <c r="O21" s="6"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -886,15 +787,9 @@
       <c r="O22" s="7"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -909,15 +804,9 @@
       <c r="O23" s="7"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -943,15 +832,9 @@
       <c r="Z24" s="18"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -977,15 +860,9 @@
       <c r="Z25" s="18"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>53</v>
-      </c>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1011,15 +888,9 @@
       <c r="Z26" s="18"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1045,15 +916,9 @@
       <c r="Z27" s="18"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1079,15 +944,9 @@
       <c r="Z28" s="19"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1113,15 +972,9 @@
       <c r="Z29" s="19"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -2765,7 +2618,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>

</xml_diff>

<commit_message>
Added new functions and test cases and test data file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Variable</t>
   </si>
@@ -35,6 +35,9 @@
     <t>URL_login_login</t>
   </si>
   <si>
+    <t>#/login</t>
+  </si>
+  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
@@ -44,9 +47,6 @@
     <t>MicrosoftInternetExplorer</t>
   </si>
   <si>
-    <t>#/login</t>
-  </si>
-  <si>
     <t>MicrosoftEdge</t>
   </si>
   <si>
@@ -129,13 +129,70 @@
   </si>
   <si>
     <t>New Dashboard</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_SharedView</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_SharedShare</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_SharedEdit</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent1</t>
+  </si>
+  <si>
+    <t>New folder</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent2</t>
+  </si>
+  <si>
+    <t>new folder inside Automation_Folder_CatalogOfContent1</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent3</t>
+  </si>
+  <si>
+    <t>new folder inside Automation_Folder_CatalogOfContent2</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_InsideNestedFolder</t>
+  </si>
+  <si>
+    <t>New Dashboard inside Automation_Folder_CatalogOfContent3</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_Arabic</t>
+  </si>
+  <si>
+    <t>كتالوج الأتمتة لمحتوى لوحة المعلومات باللغة العربية</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_SpecialCharacters</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_!@#$%^&amp;*()_+=-{}[]|</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_French</t>
+  </si>
+  <si>
+    <t>ĉĈćêĉĈćĆąăëêéèçàáéèçàá</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_Chinese</t>
+  </si>
+  <si>
+    <t>汉字汉字汉字漢字汉字</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -166,6 +223,12 @@
     <font>
       <sz val="11.0"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
     </font>
   </fonts>
   <fills count="5">
@@ -250,18 +313,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -295,14 +358,20 @@
     <xf borderId="0" fillId="4" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -368,11 +437,11 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -389,10 +458,10 @@
       <c r="O2" s="6"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="5"/>
@@ -410,10 +479,10 @@
       <c r="O3" s="7"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5"/>
@@ -431,10 +500,10 @@
       <c r="O4" s="7"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="5"/>
@@ -452,10 +521,10 @@
       <c r="O5" s="7"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5"/>
@@ -473,10 +542,10 @@
       <c r="O6" s="7"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="5"/>
@@ -494,10 +563,10 @@
       <c r="O7" s="7"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="5"/>
@@ -515,10 +584,10 @@
       <c r="O8" s="7"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="5"/>
@@ -536,10 +605,10 @@
       <c r="O9" s="7"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="5"/>
@@ -557,10 +626,10 @@
       <c r="O10" s="7"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="5"/>
@@ -597,20 +666,20 @@
       <c r="O12" s="6"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -618,20 +687,20 @@
       <c r="O13" s="7"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -639,20 +708,20 @@
       <c r="O14" s="7"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -685,7 +754,7 @@
       <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="5"/>
@@ -702,890 +771,956 @@
       <c r="O17" s="7"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="A18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
       <c r="O18" s="6"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="A19" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
       <c r="O19" s="7"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="A20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
       <c r="O20" s="7"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
+      <c r="A21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
       <c r="O21" s="6"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
+      <c r="A22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
       <c r="O22" s="7"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
       <c r="O23" s="7"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18"/>
-      <c r="Y24" s="18"/>
-      <c r="Z24" s="18"/>
+      <c r="A24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="U25" s="18"/>
-      <c r="V25" s="18"/>
-      <c r="W25" s="18"/>
-      <c r="X25" s="18"/>
-      <c r="Y25" s="18"/>
-      <c r="Z25" s="18"/>
+      <c r="A25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="18"/>
-      <c r="V26" s="18"/>
-      <c r="W26" s="18"/>
-      <c r="X26" s="18"/>
-      <c r="Y26" s="18"/>
-      <c r="Z26" s="18"/>
+      <c r="A26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="17"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
-      <c r="W27" s="18"/>
-      <c r="X27" s="18"/>
-      <c r="Y27" s="18"/>
-      <c r="Z27" s="18"/>
+      <c r="A27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="17"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
-      <c r="W28" s="19"/>
-      <c r="X28" s="19"/>
-      <c r="Y28" s="19"/>
-      <c r="Z28" s="19"/>
+      <c r="A28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="21"/>
+      <c r="Y28" s="21"/>
+      <c r="Z28" s="21"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
-      <c r="T29" s="19"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="19"/>
-      <c r="W29" s="19"/>
-      <c r="X29" s="19"/>
-      <c r="Y29" s="19"/>
-      <c r="Z29" s="19"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="21"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="21"/>
+      <c r="X29" s="21"/>
+      <c r="Y29" s="21"/>
+      <c r="Z29" s="21"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
-      <c r="W30" s="19"/>
-      <c r="X30" s="19"/>
-      <c r="Y30" s="19"/>
-      <c r="Z30" s="19"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
+      <c r="U30" s="21"/>
+      <c r="V30" s="21"/>
+      <c r="W30" s="21"/>
+      <c r="X30" s="21"/>
+      <c r="Y30" s="21"/>
+      <c r="Z30" s="21"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
-      <c r="W31" s="19"/>
-      <c r="X31" s="19"/>
-      <c r="Y31" s="19"/>
-      <c r="Z31" s="19"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="21"/>
+      <c r="Z31" s="21"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="19"/>
-      <c r="Y32" s="19"/>
-      <c r="Z32" s="19"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="21"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="3"/>
+      <c r="A33" s="2"/>
       <c r="B33" s="15"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-      <c r="W33" s="19"/>
-      <c r="X33" s="19"/>
-      <c r="Y33" s="19"/>
-      <c r="Z33" s="19"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="21"/>
+      <c r="W33" s="21"/>
+      <c r="X33" s="21"/>
+      <c r="Y33" s="21"/>
+      <c r="Z33" s="21"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19"/>
-      <c r="X34" s="19"/>
-      <c r="Y34" s="19"/>
-      <c r="Z34" s="19"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="21"/>
+      <c r="V34" s="21"/>
+      <c r="W34" s="21"/>
+      <c r="X34" s="21"/>
+      <c r="Y34" s="21"/>
+      <c r="Z34" s="21"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-      <c r="W35" s="19"/>
-      <c r="X35" s="19"/>
-      <c r="Y35" s="19"/>
-      <c r="Z35" s="19"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="21"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="21"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="21"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="21"/>
+      <c r="Z35" s="21"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19"/>
-      <c r="U36" s="19"/>
-      <c r="V36" s="19"/>
-      <c r="W36" s="19"/>
-      <c r="X36" s="19"/>
-      <c r="Y36" s="19"/>
-      <c r="Z36" s="19"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="21"/>
+      <c r="U36" s="21"/>
+      <c r="V36" s="21"/>
+      <c r="W36" s="21"/>
+      <c r="X36" s="21"/>
+      <c r="Y36" s="21"/>
+      <c r="Z36" s="21"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="19"/>
-      <c r="Y37" s="19"/>
-      <c r="Z37" s="19"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="21"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="21"/>
+      <c r="Z37" s="21"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
-      <c r="Y38" s="19"/>
-      <c r="Z38" s="19"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="21"/>
+      <c r="Z38" s="21"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
-      <c r="R39" s="19"/>
-      <c r="S39" s="19"/>
-      <c r="T39" s="19"/>
-      <c r="U39" s="19"/>
-      <c r="V39" s="19"/>
-      <c r="W39" s="19"/>
-      <c r="X39" s="19"/>
-      <c r="Y39" s="19"/>
-      <c r="Z39" s="19"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="W39" s="21"/>
+      <c r="X39" s="21"/>
+      <c r="Y39" s="21"/>
+      <c r="Z39" s="21"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="19"/>
-      <c r="R40" s="19"/>
-      <c r="S40" s="19"/>
-      <c r="T40" s="19"/>
-      <c r="U40" s="19"/>
-      <c r="V40" s="19"/>
-      <c r="W40" s="19"/>
-      <c r="X40" s="19"/>
-      <c r="Y40" s="19"/>
-      <c r="Z40" s="19"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="21"/>
+      <c r="W40" s="21"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="21"/>
+      <c r="Z40" s="21"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19"/>
-      <c r="Y41" s="19"/>
-      <c r="Z41" s="19"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
+      <c r="Z41" s="21"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19"/>
-      <c r="U42" s="19"/>
-      <c r="V42" s="19"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19"/>
-      <c r="Y42" s="19"/>
-      <c r="Z42" s="19"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="21"/>
+      <c r="R42" s="21"/>
+      <c r="S42" s="21"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="21"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="21"/>
+      <c r="Z42" s="21"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="19"/>
-      <c r="S43" s="19"/>
-      <c r="T43" s="19"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="19"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="19"/>
-      <c r="Y43" s="19"/>
-      <c r="Z43" s="19"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="21"/>
+      <c r="T43" s="21"/>
+      <c r="U43" s="21"/>
+      <c r="V43" s="21"/>
+      <c r="W43" s="21"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="21"/>
+      <c r="Z43" s="21"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19"/>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19"/>
-      <c r="Y44" s="19"/>
-      <c r="Z44" s="19"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="21"/>
+      <c r="Q44" s="21"/>
+      <c r="R44" s="21"/>
+      <c r="S44" s="21"/>
+      <c r="T44" s="21"/>
+      <c r="U44" s="21"/>
+      <c r="V44" s="21"/>
+      <c r="W44" s="21"/>
+      <c r="X44" s="21"/>
+      <c r="Y44" s="21"/>
+      <c r="Z44" s="21"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="19"/>
-      <c r="Y45" s="19"/>
-      <c r="Z45" s="19"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="21"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="21"/>
+      <c r="U45" s="21"/>
+      <c r="V45" s="21"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="21"/>
+      <c r="Z45" s="21"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="19"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
-      <c r="S46" s="19"/>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19"/>
-      <c r="Y46" s="19"/>
-      <c r="Z46" s="19"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="21"/>
+      <c r="R46" s="21"/>
+      <c r="S46" s="21"/>
+      <c r="T46" s="21"/>
+      <c r="U46" s="21"/>
+      <c r="V46" s="21"/>
+      <c r="W46" s="21"/>
+      <c r="X46" s="21"/>
+      <c r="Y46" s="21"/>
+      <c r="Z46" s="21"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="19"/>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="19"/>
-      <c r="R47" s="19"/>
-      <c r="S47" s="19"/>
-      <c r="T47" s="19"/>
-      <c r="U47" s="19"/>
-      <c r="V47" s="19"/>
-      <c r="W47" s="19"/>
-      <c r="X47" s="19"/>
-      <c r="Y47" s="19"/>
-      <c r="Z47" s="19"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="21"/>
+      <c r="P47" s="21"/>
+      <c r="Q47" s="21"/>
+      <c r="R47" s="21"/>
+      <c r="S47" s="21"/>
+      <c r="T47" s="21"/>
+      <c r="U47" s="21"/>
+      <c r="V47" s="21"/>
+      <c r="W47" s="21"/>
+      <c r="X47" s="21"/>
+      <c r="Y47" s="21"/>
+      <c r="Z47" s="21"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="19"/>
-      <c r="P48" s="19"/>
-      <c r="Q48" s="19"/>
-      <c r="R48" s="19"/>
-      <c r="S48" s="19"/>
-      <c r="T48" s="19"/>
-      <c r="U48" s="19"/>
-      <c r="V48" s="19"/>
-      <c r="W48" s="19"/>
-      <c r="X48" s="19"/>
-      <c r="Y48" s="19"/>
-      <c r="Z48" s="19"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="21"/>
+      <c r="P48" s="21"/>
+      <c r="Q48" s="21"/>
+      <c r="R48" s="21"/>
+      <c r="S48" s="21"/>
+      <c r="T48" s="21"/>
+      <c r="U48" s="21"/>
+      <c r="V48" s="21"/>
+      <c r="W48" s="21"/>
+      <c r="X48" s="21"/>
+      <c r="Y48" s="21"/>
+      <c r="Z48" s="21"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="19"/>
-      <c r="P49" s="19"/>
-      <c r="Q49" s="19"/>
-      <c r="R49" s="19"/>
-      <c r="S49" s="19"/>
-      <c r="T49" s="19"/>
-      <c r="U49" s="19"/>
-      <c r="V49" s="19"/>
-      <c r="W49" s="19"/>
-      <c r="X49" s="19"/>
-      <c r="Y49" s="19"/>
-      <c r="Z49" s="19"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="21"/>
+      <c r="P49" s="21"/>
+      <c r="Q49" s="21"/>
+      <c r="R49" s="21"/>
+      <c r="S49" s="21"/>
+      <c r="T49" s="21"/>
+      <c r="U49" s="21"/>
+      <c r="V49" s="21"/>
+      <c r="W49" s="21"/>
+      <c r="X49" s="21"/>
+      <c r="Y49" s="21"/>
+      <c r="Z49" s="21"/>
     </row>
     <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="19"/>
-      <c r="R50" s="19"/>
-      <c r="S50" s="19"/>
-      <c r="T50" s="19"/>
-      <c r="U50" s="19"/>
-      <c r="V50" s="19"/>
-      <c r="W50" s="19"/>
-      <c r="X50" s="19"/>
-      <c r="Y50" s="19"/>
-      <c r="Z50" s="19"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
+      <c r="P50" s="21"/>
+      <c r="Q50" s="21"/>
+      <c r="R50" s="21"/>
+      <c r="S50" s="21"/>
+      <c r="T50" s="21"/>
+      <c r="U50" s="21"/>
+      <c r="V50" s="21"/>
+      <c r="W50" s="21"/>
+      <c r="X50" s="21"/>
+      <c r="Y50" s="21"/>
+      <c r="Z50" s="21"/>
     </row>
     <row r="51" ht="13.5" customHeight="1">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="19"/>
-      <c r="N51" s="19"/>
-      <c r="O51" s="19"/>
-      <c r="P51" s="19"/>
-      <c r="Q51" s="19"/>
-      <c r="R51" s="19"/>
-      <c r="S51" s="19"/>
-      <c r="T51" s="19"/>
-      <c r="U51" s="19"/>
-      <c r="V51" s="19"/>
-      <c r="W51" s="19"/>
-      <c r="X51" s="19"/>
-      <c r="Y51" s="19"/>
-      <c r="Z51" s="19"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
+      <c r="P51" s="21"/>
+      <c r="Q51" s="21"/>
+      <c r="R51" s="21"/>
+      <c r="S51" s="21"/>
+      <c r="T51" s="21"/>
+      <c r="U51" s="21"/>
+      <c r="V51" s="21"/>
+      <c r="W51" s="21"/>
+      <c r="X51" s="21"/>
+      <c r="Y51" s="21"/>
+      <c r="Z51" s="21"/>
     </row>
     <row r="52" ht="15.75" customHeight="1"/>
     <row r="53" ht="15.75" customHeight="1"/>
@@ -2557,79 +2692,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
NewUI_CatalogOfContent.java - New Test cases created. NewUI_Content.java - New functions was created. catalogOfContent_newUI/TestData.xlsx - TestData file updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
   <si>
     <t>Variable</t>
   </si>
@@ -35,18 +35,18 @@
     <t>URL_login_login</t>
   </si>
   <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
     <t>#/login</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
     <t>MicrosoftEdge</t>
   </si>
   <si>
@@ -134,6 +134,9 @@
     <t>Automation_Dashboard_CatalogOfContent_SharedView</t>
   </si>
   <si>
+    <t>New Dashboard Created by admin and shared</t>
+  </si>
+  <si>
     <t>Automation_Dashboard_CatalogOfContent_SharedShare</t>
   </si>
   <si>
@@ -186,6 +189,87 @@
   </si>
   <si>
     <t>汉字汉字汉字漢字汉字</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_Deleted</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_NotShared</t>
+  </si>
+  <si>
+    <t>New Dashboard Created by admin and not shared</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_DashboardNotCreated</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_SharedView</t>
+  </si>
+  <si>
+    <t>New Folder Created by admin and shared</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_SharedShare</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_SharedEdit</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent1.1</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent2.1</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent3.1</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_InsideNestedFolder</t>
+  </si>
+  <si>
+    <t>New Folder inside Automation_Folder_CatalogOfContent3</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_Arabic</t>
+  </si>
+  <si>
+    <t>كتالوج الأتمتة لمحتوى لوحة المعلومات باللغة العربيةFolder_Content_</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_SpecialCharacters</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_!@#$%^&amp;*()_+=-{}[]|</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_French</t>
+  </si>
+  <si>
+    <t>Folder_Content_ĉĈćêĉĈćĆąăëêéèçàáéèçàá</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_Chinese</t>
+  </si>
+  <si>
+    <t>Folder_Content_汉字汉字汉字漢字汉字</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_Deleted</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_NotShared</t>
+  </si>
+  <si>
+    <t>New Folder Created by admin and not shared</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_FolderNotCreated</t>
+  </si>
+  <si>
+    <t>Folder name which will not be created</t>
   </si>
 </sst>
 </file>
@@ -320,11 +404,11 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -404,7 +488,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="58.43"/>
     <col customWidth="1" min="2" max="2" width="64.29"/>
-    <col customWidth="1" min="3" max="3" width="36.14"/>
+    <col customWidth="1" min="3" max="3" width="48.43"/>
     <col customWidth="1" min="4" max="15" width="8.57"/>
     <col customWidth="1" min="16" max="26" width="8.71"/>
   </cols>
@@ -437,11 +521,11 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -458,10 +542,10 @@
       <c r="O2" s="6"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="5"/>
@@ -479,10 +563,10 @@
       <c r="O3" s="7"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5"/>
@@ -500,10 +584,10 @@
       <c r="O4" s="7"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="5"/>
@@ -521,10 +605,10 @@
       <c r="O5" s="7"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5"/>
@@ -542,10 +626,10 @@
       <c r="O6" s="7"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="5"/>
@@ -563,10 +647,10 @@
       <c r="O7" s="7"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="5"/>
@@ -584,10 +668,10 @@
       <c r="O8" s="7"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="5"/>
@@ -605,10 +689,10 @@
       <c r="O9" s="7"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="5"/>
@@ -626,10 +710,10 @@
       <c r="O10" s="7"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="5"/>
@@ -666,20 +750,20 @@
       <c r="O12" s="6"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -687,20 +771,20 @@
       <c r="O13" s="7"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -708,20 +792,20 @@
       <c r="O14" s="7"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -754,7 +838,7 @@
       <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="5"/>
@@ -777,158 +861,158 @@
       <c r="B18" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
       <c r="O18" s="6"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
       <c r="O19" s="7"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
       <c r="O20" s="7"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
+      <c r="C21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
       <c r="O21" s="6"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
+      <c r="C22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
       <c r="O22" s="7"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
+      <c r="B23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
       <c r="O23" s="7"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
+      <c r="C24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
       <c r="O24" s="16"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="17"/>
@@ -944,25 +1028,25 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
       <c r="O25" s="16"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="17"/>
@@ -978,25 +1062,25 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
       <c r="O26" s="16"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="17"/>
@@ -1012,25 +1096,25 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
       <c r="O27" s="16"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="17"/>
@@ -1046,25 +1130,25 @@
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
       <c r="O28" s="21"/>
       <c r="P28" s="21"/>
       <c r="Q28" s="21"/>
@@ -1079,20 +1163,26 @@
       <c r="Z28" s="21"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="A29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
       <c r="O29" s="21"/>
       <c r="P29" s="21"/>
       <c r="Q29" s="21"/>
@@ -1107,20 +1197,26 @@
       <c r="Z29" s="21"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="A30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
       <c r="O30" s="21"/>
       <c r="P30" s="21"/>
       <c r="Q30" s="21"/>
@@ -1135,20 +1231,26 @@
       <c r="Z30" s="21"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="A31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
       <c r="O31" s="21"/>
       <c r="P31" s="21"/>
       <c r="Q31" s="21"/>
@@ -1163,48 +1265,45 @@
       <c r="Z31" s="21"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="21"/>
-      <c r="V32" s="21"/>
-      <c r="W32" s="21"/>
-      <c r="X32" s="21"/>
-      <c r="Y32" s="21"/>
-      <c r="Z32" s="21"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="2"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="A33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
       <c r="O33" s="21"/>
       <c r="P33" s="21"/>
       <c r="Q33" s="21"/>
@@ -1219,20 +1318,26 @@
       <c r="Z33" s="21"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+      <c r="A34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
       <c r="O34" s="21"/>
       <c r="P34" s="21"/>
       <c r="Q34" s="21"/>
@@ -1247,20 +1352,26 @@
       <c r="Z34" s="21"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+      <c r="A35" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
       <c r="O35" s="21"/>
       <c r="P35" s="21"/>
       <c r="Q35" s="21"/>
@@ -1275,20 +1386,26 @@
       <c r="Z35" s="21"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="A36" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
       <c r="O36" s="21"/>
       <c r="P36" s="21"/>
       <c r="Q36" s="21"/>
@@ -1303,20 +1420,26 @@
       <c r="Z36" s="21"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+      <c r="A37" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
       <c r="O37" s="21"/>
       <c r="P37" s="21"/>
       <c r="Q37" s="21"/>
@@ -1331,20 +1454,26 @@
       <c r="Z37" s="21"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
+      <c r="A38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
       <c r="O38" s="21"/>
       <c r="P38" s="21"/>
       <c r="Q38" s="21"/>
@@ -1359,20 +1488,26 @@
       <c r="Z38" s="21"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
       <c r="O39" s="21"/>
       <c r="P39" s="21"/>
       <c r="Q39" s="21"/>
@@ -1387,20 +1522,26 @@
       <c r="Z39" s="21"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="A40" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
       <c r="O40" s="21"/>
       <c r="P40" s="21"/>
       <c r="Q40" s="21"/>
@@ -1415,20 +1556,26 @@
       <c r="Z40" s="21"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+      <c r="A41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
       <c r="O41" s="21"/>
       <c r="P41" s="21"/>
       <c r="Q41" s="21"/>
@@ -1443,20 +1590,26 @@
       <c r="Z41" s="21"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
+      <c r="A42" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
       <c r="O42" s="21"/>
       <c r="P42" s="21"/>
       <c r="Q42" s="21"/>
@@ -1471,20 +1624,26 @@
       <c r="Z42" s="21"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
+      <c r="A43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
       <c r="O43" s="21"/>
       <c r="P43" s="21"/>
       <c r="Q43" s="21"/>
@@ -1499,20 +1658,26 @@
       <c r="Z43" s="21"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+      <c r="A44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
       <c r="O44" s="21"/>
       <c r="P44" s="21"/>
       <c r="Q44" s="21"/>
@@ -1527,20 +1692,26 @@
       <c r="Z44" s="21"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+      <c r="A45" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
       <c r="O45" s="21"/>
       <c r="P45" s="21"/>
       <c r="Q45" s="21"/>
@@ -1555,20 +1726,26 @@
       <c r="Z45" s="21"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
+      <c r="A46" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
       <c r="O46" s="21"/>
       <c r="P46" s="21"/>
       <c r="Q46" s="21"/>
@@ -1583,20 +1760,26 @@
       <c r="Z46" s="21"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
+      <c r="A47" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
       <c r="O47" s="21"/>
       <c r="P47" s="21"/>
       <c r="Q47" s="21"/>
@@ -1611,20 +1794,20 @@
       <c r="Z47" s="21"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
       <c r="O48" s="21"/>
       <c r="P48" s="21"/>
       <c r="Q48" s="21"/>
@@ -1639,20 +1822,20 @@
       <c r="Z48" s="21"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
       <c r="O49" s="21"/>
       <c r="P49" s="21"/>
       <c r="Q49" s="21"/>
@@ -2692,79 +2875,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added new test cases with functions and test data file.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
   <si>
     <t>Variable</t>
   </si>
@@ -270,6 +270,24 @@
   </si>
   <si>
     <t>Folder name which will not be created</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_DashboardDetailsSection</t>
+  </si>
+  <si>
+    <t>New Dashboard with below description</t>
+  </si>
+  <si>
+    <t>This information is for Automation testing purposes.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_DashboardDetailsSection_OwnedBy</t>
+  </si>
+  <si>
+    <t>New Dashboard Created by user to check that it's owned by this user</t>
   </si>
 </sst>
 </file>
@@ -1794,9 +1812,15 @@
       <c r="Z47" s="21"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+      <c r="A48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -1822,9 +1846,15 @@
       <c r="Z48" s="21"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+      <c r="A49" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -1850,9 +1880,15 @@
       <c r="Z49" s="21"/>
     </row>
     <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="21"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
+      <c r="A50" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21"/>
       <c r="F50" s="21"/>
@@ -1878,9 +1914,9 @@
       <c r="Z50" s="21"/>
     </row>
     <row r="51" ht="13.5" customHeight="1">
-      <c r="A51" s="21"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
       <c r="D51" s="21"/>
       <c r="E51" s="21"/>
       <c r="F51" s="21"/>
@@ -1905,7 +1941,11 @@
       <c r="Y51" s="21"/>
       <c r="Z51" s="21"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+    </row>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1"/>
     <row r="55" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added new Test cases and functions and tets data.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="95">
   <si>
     <t>Variable</t>
   </si>
@@ -41,12 +41,12 @@
     <t>GoogleChrome</t>
   </si>
   <si>
+    <t>#/login</t>
+  </si>
+  <si>
     <t>MicrosoftInternetExplorer</t>
   </si>
   <si>
-    <t>#/login</t>
-  </si>
-  <si>
     <t>MicrosoftEdge</t>
   </si>
   <si>
@@ -272,7 +272,7 @@
     <t>Folder name which will not be created</t>
   </si>
   <si>
-    <t>Automation_Folder_CatalogOfContent_DashboardDetailsSection</t>
+    <t>Automation_Dashboard_CatalogOfContent_DashboardDetailsSection</t>
   </si>
   <si>
     <t>New Dashboard with below description</t>
@@ -284,10 +284,19 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Automation_Folder_CatalogOfContent_DashboardDetailsSection_OwnedBy</t>
-  </si>
-  <si>
-    <t>New Dashboard Created by user to check that it's owned by this user</t>
+    <t>Automation_Dashboard_CatalogOfContent_DashboardDetailsSection_ModifiedBy</t>
+  </si>
+  <si>
+    <t>New Dashboard Created by Admin and shared edit to analyzer with insight created without name</t>
+  </si>
+  <si>
+    <t>InsightName</t>
+  </si>
+  <si>
+    <t>Automation_InsightName</t>
+  </si>
+  <si>
+    <t>New Insight Name</t>
   </si>
 </sst>
 </file>
@@ -415,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -478,6 +487,9 @@
     <xf borderId="5" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -543,7 +555,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1811,7 +1823,7 @@
       <c r="Y47" s="21"/>
       <c r="Z47" s="21"/>
     </row>
-    <row r="48" ht="13.5" customHeight="1">
+    <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>86</v>
       </c>
@@ -1846,105 +1858,102 @@
       <c r="Z48" s="21"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="21"/>
-      <c r="P49" s="21"/>
-      <c r="Q49" s="21"/>
-      <c r="R49" s="21"/>
-      <c r="S49" s="21"/>
-      <c r="T49" s="21"/>
-      <c r="U49" s="21"/>
-      <c r="V49" s="21"/>
-      <c r="W49" s="21"/>
-      <c r="X49" s="21"/>
-      <c r="Y49" s="21"/>
-      <c r="Z49" s="21"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
     </row>
     <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="21"/>
-      <c r="N50" s="21"/>
-      <c r="O50" s="21"/>
-      <c r="P50" s="21"/>
-      <c r="Q50" s="21"/>
-      <c r="R50" s="21"/>
-      <c r="S50" s="21"/>
-      <c r="T50" s="21"/>
-      <c r="U50" s="21"/>
-      <c r="V50" s="21"/>
-      <c r="W50" s="21"/>
-      <c r="X50" s="21"/>
-      <c r="Y50" s="21"/>
-      <c r="Z50" s="21"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
     </row>
     <row r="51" ht="13.5" customHeight="1">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="21"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="21"/>
-      <c r="S51" s="21"/>
-      <c r="T51" s="21"/>
-      <c r="U51" s="21"/>
-      <c r="V51" s="21"/>
-      <c r="W51" s="21"/>
-      <c r="X51" s="21"/>
-      <c r="Y51" s="21"/>
-      <c r="Z51" s="21"/>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="19"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1"/>
@@ -2961,7 +2970,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>

</xml_diff>

<commit_message>
Added new test cases, functions and test data. updated login function with assertion.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,14 +12,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="104">
+  <si>
+    <t>Supported Browser Types</t>
+  </si>
+  <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
+  </si>
   <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -32,24 +44,15 @@
     <t>Data4</t>
   </si>
   <si>
+    <t>Data5</t>
+  </si>
+  <si>
     <t>URL_login_login</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
     <t>#/login</t>
   </si>
   <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>URL_content</t>
   </si>
   <si>
@@ -116,6 +119,18 @@
     <t>Automation_Analyzer</t>
   </si>
   <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Automation_Individual</t>
+  </si>
+  <si>
+    <t>Automation_SchemaManager</t>
+  </si>
+  <si>
+    <t>Automation_User</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
@@ -297,6 +312,18 @@
   </si>
   <si>
     <t>New Insight Name</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_TestingSearchWithAllUsers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Dashboard Created By admin and shared with all users </t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_TestingSearchWithAllUsers</t>
+  </si>
+  <si>
+    <t>New Folder Created by Admin and shared with all users</t>
   </si>
 </sst>
 </file>
@@ -424,15 +451,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -519,1444 +549,1493 @@
     <col customWidth="1" min="1" max="1" width="58.43"/>
     <col customWidth="1" min="2" max="2" width="64.29"/>
     <col customWidth="1" min="3" max="3" width="48.43"/>
-    <col customWidth="1" min="4" max="15" width="8.57"/>
+    <col customWidth="1" min="4" max="4" width="21.71"/>
+    <col customWidth="1" min="5" max="5" width="27.43"/>
+    <col customWidth="1" min="6" max="6" width="16.86"/>
+    <col customWidth="1" min="7" max="15" width="8.57"/>
     <col customWidth="1" min="16" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="A12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
+      <c r="D15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
+      <c r="A17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="6"/>
+      <c r="A18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="7"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="8"/>
+    </row>
+    <row r="20" ht="13.5" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="8"/>
+    </row>
+    <row r="21" ht="13.5" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" ht="13.5" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="8"/>
+    </row>
+    <row r="23" ht="13.5" customHeight="1">
+      <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="8"/>
+    </row>
+    <row r="24" ht="13.5" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="18"/>
+      <c r="V24" s="18"/>
+      <c r="W24" s="18"/>
+      <c r="X24" s="18"/>
+      <c r="Y24" s="18"/>
+      <c r="Z24" s="18"/>
+    </row>
+    <row r="25" ht="13.5" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="18"/>
+      <c r="V25" s="18"/>
+      <c r="W25" s="18"/>
+      <c r="X25" s="18"/>
+      <c r="Y25" s="18"/>
+      <c r="Z25" s="18"/>
+    </row>
+    <row r="26" ht="13.5" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="18"/>
+      <c r="U26" s="18"/>
+      <c r="V26" s="18"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="18"/>
+      <c r="Z26" s="18"/>
+    </row>
+    <row r="27" ht="13.5" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
+      <c r="V27" s="18"/>
+      <c r="W27" s="18"/>
+      <c r="X27" s="18"/>
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="18"/>
+    </row>
+    <row r="28" ht="13.5" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22"/>
+      <c r="Z28" s="22"/>
+    </row>
+    <row r="29" ht="13.5" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+    </row>
+    <row r="30" ht="13.5" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+      <c r="U30" s="22"/>
+      <c r="V30" s="22"/>
+      <c r="W30" s="22"/>
+      <c r="X30" s="22"/>
+      <c r="Y30" s="22"/>
+      <c r="Z30" s="22"/>
+    </row>
+    <row r="31" ht="13.5" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="22"/>
+      <c r="V31" s="22"/>
+      <c r="W31" s="22"/>
+      <c r="X31" s="22"/>
+      <c r="Y31" s="22"/>
+      <c r="Z31" s="22"/>
+    </row>
+    <row r="32" ht="13.5" customHeight="1">
+      <c r="A32" s="9"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" ht="13.5" customHeight="1">
+      <c r="A33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="22"/>
+      <c r="X33" s="22"/>
+      <c r="Y33" s="22"/>
+      <c r="Z33" s="22"/>
+    </row>
+    <row r="34" ht="13.5" customHeight="1">
+      <c r="A34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="22"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="22"/>
+      <c r="X34" s="22"/>
+      <c r="Y34" s="22"/>
+      <c r="Z34" s="22"/>
+    </row>
+    <row r="35" ht="13.5" customHeight="1">
+      <c r="A35" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="22"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
+      <c r="X35" s="22"/>
+      <c r="Y35" s="22"/>
+      <c r="Z35" s="22"/>
+    </row>
+    <row r="36" ht="13.5" customHeight="1">
+      <c r="A36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="22"/>
+      <c r="X36" s="22"/>
+      <c r="Y36" s="22"/>
+      <c r="Z36" s="22"/>
+    </row>
+    <row r="37" ht="13.5" customHeight="1">
+      <c r="A37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="22"/>
+      <c r="X37" s="22"/>
+      <c r="Y37" s="22"/>
+      <c r="Z37" s="22"/>
+    </row>
+    <row r="38" ht="13.5" customHeight="1">
+      <c r="A38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+      <c r="U38" s="22"/>
+      <c r="V38" s="22"/>
+      <c r="W38" s="22"/>
+      <c r="X38" s="22"/>
+      <c r="Y38" s="22"/>
+      <c r="Z38" s="22"/>
+    </row>
+    <row r="39" ht="13.5" customHeight="1">
+      <c r="A39" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="22"/>
+      <c r="R39" s="22"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
+      <c r="U39" s="22"/>
+      <c r="V39" s="22"/>
+      <c r="W39" s="22"/>
+      <c r="X39" s="22"/>
+      <c r="Y39" s="22"/>
+      <c r="Z39" s="22"/>
+    </row>
+    <row r="40" ht="13.5" customHeight="1">
+      <c r="A40" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="22"/>
+      <c r="P40" s="22"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
+      <c r="U40" s="22"/>
+      <c r="V40" s="22"/>
+      <c r="W40" s="22"/>
+      <c r="X40" s="22"/>
+      <c r="Y40" s="22"/>
+      <c r="Z40" s="22"/>
+    </row>
+    <row r="41" ht="13.5" customHeight="1">
+      <c r="A41" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="22"/>
+      <c r="P41" s="22"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="22"/>
+      <c r="S41" s="22"/>
+      <c r="T41" s="22"/>
+      <c r="U41" s="22"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="22"/>
+      <c r="X41" s="22"/>
+      <c r="Y41" s="22"/>
+      <c r="Z41" s="22"/>
+    </row>
+    <row r="42" ht="13.5" customHeight="1">
+      <c r="A42" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="22"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
+      <c r="U42" s="22"/>
+      <c r="V42" s="22"/>
+      <c r="W42" s="22"/>
+      <c r="X42" s="22"/>
+      <c r="Y42" s="22"/>
+      <c r="Z42" s="22"/>
+    </row>
+    <row r="43" ht="13.5" customHeight="1">
+      <c r="A43" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="22"/>
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="22"/>
+      <c r="U43" s="22"/>
+      <c r="V43" s="22"/>
+      <c r="W43" s="22"/>
+      <c r="X43" s="22"/>
+      <c r="Y43" s="22"/>
+      <c r="Z43" s="22"/>
+    </row>
+    <row r="44" ht="13.5" customHeight="1">
+      <c r="A44" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="22"/>
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="22"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="22"/>
+      <c r="U44" s="22"/>
+      <c r="V44" s="22"/>
+      <c r="W44" s="22"/>
+      <c r="X44" s="22"/>
+      <c r="Y44" s="22"/>
+      <c r="Z44" s="22"/>
+    </row>
+    <row r="45" ht="13.5" customHeight="1">
+      <c r="A45" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="22"/>
+      <c r="P45" s="22"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="22"/>
+      <c r="S45" s="22"/>
+      <c r="T45" s="22"/>
+      <c r="U45" s="22"/>
+      <c r="V45" s="22"/>
+      <c r="W45" s="22"/>
+      <c r="X45" s="22"/>
+      <c r="Y45" s="22"/>
+      <c r="Z45" s="22"/>
+    </row>
+    <row r="46" ht="13.5" customHeight="1">
+      <c r="A46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="22"/>
+      <c r="P46" s="22"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
+      <c r="T46" s="22"/>
+      <c r="U46" s="22"/>
+      <c r="V46" s="22"/>
+      <c r="W46" s="22"/>
+      <c r="X46" s="22"/>
+      <c r="Y46" s="22"/>
+      <c r="Z46" s="22"/>
+    </row>
+    <row r="47" ht="13.5" customHeight="1">
+      <c r="A47" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="22"/>
+      <c r="P47" s="22"/>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="22"/>
+      <c r="S47" s="22"/>
+      <c r="T47" s="22"/>
+      <c r="U47" s="22"/>
+      <c r="V47" s="22"/>
+      <c r="W47" s="22"/>
+      <c r="X47" s="22"/>
+      <c r="Y47" s="22"/>
+      <c r="Z47" s="22"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="22"/>
+      <c r="P48" s="22"/>
+      <c r="Q48" s="22"/>
+      <c r="R48" s="22"/>
+      <c r="S48" s="22"/>
+      <c r="T48" s="22"/>
+      <c r="U48" s="22"/>
+      <c r="V48" s="22"/>
+      <c r="W48" s="22"/>
+      <c r="X48" s="22"/>
+      <c r="Y48" s="22"/>
+      <c r="Z48" s="22"/>
+    </row>
+    <row r="49" ht="13.5" customHeight="1">
+      <c r="A49" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="5"/>
+    </row>
+    <row r="50" ht="13.5" customHeight="1">
+      <c r="A50" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5"/>
+      <c r="W50" s="5"/>
+      <c r="X50" s="5"/>
+      <c r="Y50" s="5"/>
+      <c r="Z50" s="5"/>
+    </row>
+    <row r="51" ht="13.5" customHeight="1">
+      <c r="A51" s="9"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="7"/>
-    </row>
-    <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="7"/>
-    </row>
-    <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="6"/>
-    </row>
-    <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="7"/>
-    </row>
-    <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="7"/>
-    </row>
-    <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="17"/>
-      <c r="V24" s="17"/>
-      <c r="W24" s="17"/>
-      <c r="X24" s="17"/>
-      <c r="Y24" s="17"/>
-      <c r="Z24" s="17"/>
-    </row>
-    <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="17"/>
-      <c r="V25" s="17"/>
-      <c r="W25" s="17"/>
-      <c r="X25" s="17"/>
-      <c r="Y25" s="17"/>
-      <c r="Z25" s="17"/>
-    </row>
-    <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
-      <c r="U26" s="17"/>
-      <c r="V26" s="17"/>
-      <c r="W26" s="17"/>
-      <c r="X26" s="17"/>
-      <c r="Y26" s="17"/>
-      <c r="Z26" s="17"/>
-    </row>
-    <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="17"/>
-      <c r="V27" s="17"/>
-      <c r="W27" s="17"/>
-      <c r="X27" s="17"/>
-      <c r="Y27" s="17"/>
-      <c r="Z27" s="17"/>
-    </row>
-    <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="21"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="21"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
-      <c r="U28" s="21"/>
-      <c r="V28" s="21"/>
-      <c r="W28" s="21"/>
-      <c r="X28" s="21"/>
-      <c r="Y28" s="21"/>
-      <c r="Z28" s="21"/>
-    </row>
-    <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
-      <c r="U29" s="21"/>
-      <c r="V29" s="21"/>
-      <c r="W29" s="21"/>
-      <c r="X29" s="21"/>
-      <c r="Y29" s="21"/>
-      <c r="Z29" s="21"/>
-    </row>
-    <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="21"/>
-      <c r="S30" s="21"/>
-      <c r="T30" s="21"/>
-      <c r="U30" s="21"/>
-      <c r="V30" s="21"/>
-      <c r="W30" s="21"/>
-      <c r="X30" s="21"/>
-      <c r="Y30" s="21"/>
-      <c r="Z30" s="21"/>
-    </row>
-    <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
-      <c r="U31" s="21"/>
-      <c r="V31" s="21"/>
-      <c r="W31" s="21"/>
-      <c r="X31" s="21"/>
-      <c r="Y31" s="21"/>
-      <c r="Z31" s="21"/>
-    </row>
-    <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="8"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-    </row>
-    <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="21"/>
-      <c r="X33" s="21"/>
-      <c r="Y33" s="21"/>
-      <c r="Z33" s="21"/>
-    </row>
-    <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="21"/>
-      <c r="V34" s="21"/>
-      <c r="W34" s="21"/>
-      <c r="X34" s="21"/>
-      <c r="Y34" s="21"/>
-      <c r="Z34" s="21"/>
-    </row>
-    <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="21"/>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="21"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
-      <c r="U35" s="21"/>
-      <c r="V35" s="21"/>
-      <c r="W35" s="21"/>
-      <c r="X35" s="21"/>
-      <c r="Y35" s="21"/>
-      <c r="Z35" s="21"/>
-    </row>
-    <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="21"/>
-      <c r="P36" s="21"/>
-      <c r="Q36" s="21"/>
-      <c r="R36" s="21"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-      <c r="U36" s="21"/>
-      <c r="V36" s="21"/>
-      <c r="W36" s="21"/>
-      <c r="X36" s="21"/>
-      <c r="Y36" s="21"/>
-      <c r="Z36" s="21"/>
-    </row>
-    <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="21"/>
-      <c r="R37" s="21"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="21"/>
-      <c r="V37" s="21"/>
-      <c r="W37" s="21"/>
-      <c r="X37" s="21"/>
-      <c r="Y37" s="21"/>
-      <c r="Z37" s="21"/>
-    </row>
-    <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="21"/>
-      <c r="P38" s="21"/>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="21"/>
-      <c r="S38" s="21"/>
-      <c r="T38" s="21"/>
-      <c r="U38" s="21"/>
-      <c r="V38" s="21"/>
-      <c r="W38" s="21"/>
-      <c r="X38" s="21"/>
-      <c r="Y38" s="21"/>
-      <c r="Z38" s="21"/>
-    </row>
-    <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="21"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-      <c r="V39" s="21"/>
-      <c r="W39" s="21"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
-      <c r="Z39" s="21"/>
-    </row>
-    <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21"/>
-      <c r="R40" s="21"/>
-      <c r="S40" s="21"/>
-      <c r="T40" s="21"/>
-      <c r="U40" s="21"/>
-      <c r="V40" s="21"/>
-      <c r="W40" s="21"/>
-      <c r="X40" s="21"/>
-      <c r="Y40" s="21"/>
-      <c r="Z40" s="21"/>
-    </row>
-    <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="21"/>
-      <c r="T41" s="21"/>
-      <c r="U41" s="21"/>
-      <c r="V41" s="21"/>
-      <c r="W41" s="21"/>
-      <c r="X41" s="21"/>
-      <c r="Y41" s="21"/>
-      <c r="Z41" s="21"/>
-    </row>
-    <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="21"/>
-      <c r="P42" s="21"/>
-      <c r="Q42" s="21"/>
-      <c r="R42" s="21"/>
-      <c r="S42" s="21"/>
-      <c r="T42" s="21"/>
-      <c r="U42" s="21"/>
-      <c r="V42" s="21"/>
-      <c r="W42" s="21"/>
-      <c r="X42" s="21"/>
-      <c r="Y42" s="21"/>
-      <c r="Z42" s="21"/>
-    </row>
-    <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="21"/>
-      <c r="P43" s="21"/>
-      <c r="Q43" s="21"/>
-      <c r="R43" s="21"/>
-      <c r="S43" s="21"/>
-      <c r="T43" s="21"/>
-      <c r="U43" s="21"/>
-      <c r="V43" s="21"/>
-      <c r="W43" s="21"/>
-      <c r="X43" s="21"/>
-      <c r="Y43" s="21"/>
-      <c r="Z43" s="21"/>
-    </row>
-    <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="21"/>
-      <c r="P44" s="21"/>
-      <c r="Q44" s="21"/>
-      <c r="R44" s="21"/>
-      <c r="S44" s="21"/>
-      <c r="T44" s="21"/>
-      <c r="U44" s="21"/>
-      <c r="V44" s="21"/>
-      <c r="W44" s="21"/>
-      <c r="X44" s="21"/>
-      <c r="Y44" s="21"/>
-      <c r="Z44" s="21"/>
-    </row>
-    <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="21"/>
-      <c r="P45" s="21"/>
-      <c r="Q45" s="21"/>
-      <c r="R45" s="21"/>
-      <c r="S45" s="21"/>
-      <c r="T45" s="21"/>
-      <c r="U45" s="21"/>
-      <c r="V45" s="21"/>
-      <c r="W45" s="21"/>
-      <c r="X45" s="21"/>
-      <c r="Y45" s="21"/>
-      <c r="Z45" s="21"/>
-    </row>
-    <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="21"/>
-      <c r="P46" s="21"/>
-      <c r="Q46" s="21"/>
-      <c r="R46" s="21"/>
-      <c r="S46" s="21"/>
-      <c r="T46" s="21"/>
-      <c r="U46" s="21"/>
-      <c r="V46" s="21"/>
-      <c r="W46" s="21"/>
-      <c r="X46" s="21"/>
-      <c r="Y46" s="21"/>
-      <c r="Z46" s="21"/>
-    </row>
-    <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="21"/>
-      <c r="P47" s="21"/>
-      <c r="Q47" s="21"/>
-      <c r="R47" s="21"/>
-      <c r="S47" s="21"/>
-      <c r="T47" s="21"/>
-      <c r="U47" s="21"/>
-      <c r="V47" s="21"/>
-      <c r="W47" s="21"/>
-      <c r="X47" s="21"/>
-      <c r="Y47" s="21"/>
-      <c r="Z47" s="21"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="21"/>
-      <c r="P48" s="21"/>
-      <c r="Q48" s="21"/>
-      <c r="R48" s="21"/>
-      <c r="S48" s="21"/>
-      <c r="T48" s="21"/>
-      <c r="U48" s="21"/>
-      <c r="V48" s="21"/>
-      <c r="W48" s="21"/>
-      <c r="X48" s="21"/>
-      <c r="Y48" s="21"/>
-      <c r="Z48" s="21"/>
-    </row>
-    <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
-      <c r="W49" s="4"/>
-      <c r="X49" s="4"/>
-      <c r="Y49" s="4"/>
-      <c r="Z49" s="4"/>
-    </row>
-    <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
-      <c r="S50" s="4"/>
-      <c r="T50" s="4"/>
-      <c r="U50" s="4"/>
-      <c r="V50" s="4"/>
-      <c r="W50" s="4"/>
-      <c r="X50" s="4"/>
-      <c r="Y50" s="4"/>
-      <c r="Z50" s="4"/>
-    </row>
-    <row r="51" ht="13.5" customHeight="1">
-      <c r="A51" s="8"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
     </row>
     <row r="52">
-      <c r="A52" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B52" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
+      <c r="A52" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="55" ht="15.75" customHeight="1"/>
     <row r="56" ht="15.75" customHeight="1"/>
     <row r="57" ht="15.75" customHeight="1"/>
@@ -2924,79 +3003,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added new TCs and functions.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,11 +12,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>Data5</t>
+  </si>
+  <si>
+    <t>Data6</t>
+  </si>
+  <si>
+    <t>URL_login_login</t>
+  </si>
+  <si>
+    <t>#/login</t>
+  </si>
   <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
+    <t>URL_content</t>
+  </si>
+  <si>
+    <t>#/catalog</t>
+  </si>
+  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
@@ -29,36 +62,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>Data5</t>
-  </si>
-  <si>
-    <t>URL_login_login</t>
-  </si>
-  <si>
-    <t>#/login</t>
-  </si>
-  <si>
-    <t>URL_content</t>
-  </si>
-  <si>
-    <t>#/catalog</t>
-  </si>
-  <si>
     <t>URL_content_allContent</t>
   </si>
   <si>
@@ -131,6 +134,9 @@
     <t>Automation_User</t>
   </si>
   <si>
+    <t>UserWithProfilePicture</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
@@ -324,6 +330,18 @@
   </si>
   <si>
     <t>New Folder Created by Admin and shared with all users</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_ProfilePicture</t>
+  </si>
+  <si>
+    <t>New Folder Created by user "UserWithProfilePicture"</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_ProfilePicture</t>
+  </si>
+  <si>
+    <t>New Dashboard Created by user "UserWithProfilePicture"</t>
   </si>
 </sst>
 </file>
@@ -455,9 +473,6 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -474,6 +489,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -517,8 +535,8 @@
     <xf borderId="5" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,247 +575,249 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" ht="13.5" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-    </row>
-    <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
@@ -811,93 +831,99 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="F14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
     </row>
@@ -905,7 +931,7 @@
       <c r="A16" s="9"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
@@ -917,191 +943,191 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="5" t="s">
-        <v>44</v>
+      <c r="A18" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="6"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
       <c r="O19" s="8"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
       <c r="O20" s="8"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="7"/>
+      <c r="A21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="6"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>50</v>
+      <c r="A22" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
       <c r="O22" s="8"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
+      <c r="A23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
       <c r="O23" s="8"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="5" t="s">
-        <v>54</v>
+      <c r="A24" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
+        <v>56</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
       <c r="O24" s="17"/>
       <c r="P24" s="18"/>
       <c r="Q24" s="18"/>
@@ -1116,26 +1142,26 @@
       <c r="Z24" s="18"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>56</v>
+      <c r="A25" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
       <c r="O25" s="17"/>
       <c r="P25" s="18"/>
       <c r="Q25" s="18"/>
@@ -1150,26 +1176,26 @@
       <c r="Z25" s="18"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="5" t="s">
-        <v>58</v>
+      <c r="A26" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
       <c r="O26" s="17"/>
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
@@ -1184,26 +1210,26 @@
       <c r="Z26" s="18"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>60</v>
+      <c r="A27" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
       <c r="O27" s="17"/>
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
@@ -1218,26 +1244,26 @@
       <c r="Z27" s="18"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="5" t="s">
-        <v>62</v>
+      <c r="A28" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
       <c r="O28" s="22"/>
       <c r="P28" s="22"/>
       <c r="Q28" s="22"/>
@@ -1252,26 +1278,26 @@
       <c r="Z28" s="22"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="A29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
       <c r="O29" s="22"/>
       <c r="P29" s="22"/>
       <c r="Q29" s="22"/>
@@ -1286,26 +1312,26 @@
       <c r="Z29" s="22"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
+      <c r="A30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="22"/>
@@ -1320,26 +1346,26 @@
       <c r="Z30" s="22"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>67</v>
+      <c r="A31" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
       <c r="O31" s="22"/>
       <c r="P31" s="22"/>
       <c r="Q31" s="22"/>
@@ -1357,7 +1383,7 @@
       <c r="A32" s="9"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
@@ -1369,30 +1395,30 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
+      <c r="A33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
       <c r="O33" s="22"/>
       <c r="P33" s="22"/>
       <c r="Q33" s="22"/>
@@ -1407,26 +1433,26 @@
       <c r="Z33" s="22"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="5" t="s">
-        <v>69</v>
+      <c r="A34" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
       <c r="O34" s="22"/>
       <c r="P34" s="22"/>
       <c r="Q34" s="22"/>
@@ -1442,25 +1468,25 @@
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
       <c r="O35" s="22"/>
       <c r="P35" s="22"/>
       <c r="Q35" s="22"/>
@@ -1475,26 +1501,26 @@
       <c r="Z35" s="22"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
       <c r="O36" s="22"/>
       <c r="P36" s="22"/>
       <c r="Q36" s="22"/>
@@ -1509,26 +1535,26 @@
       <c r="Z36" s="22"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
+      <c r="A37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
       <c r="O37" s="22"/>
       <c r="P37" s="22"/>
       <c r="Q37" s="22"/>
@@ -1543,26 +1569,26 @@
       <c r="Z37" s="22"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="5" t="s">
-        <v>50</v>
+      <c r="A38" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
       <c r="O38" s="22"/>
       <c r="P38" s="22"/>
       <c r="Q38" s="22"/>
@@ -1577,26 +1603,26 @@
       <c r="Z38" s="22"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
+      <c r="A39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
       <c r="O39" s="22"/>
       <c r="P39" s="22"/>
       <c r="Q39" s="22"/>
@@ -1611,26 +1637,26 @@
       <c r="Z39" s="22"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="5" t="s">
-        <v>76</v>
+      <c r="A40" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
       <c r="O40" s="22"/>
       <c r="P40" s="22"/>
       <c r="Q40" s="22"/>
@@ -1645,26 +1671,26 @@
       <c r="Z40" s="22"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="5" t="s">
-        <v>78</v>
+      <c r="A41" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
       <c r="O41" s="22"/>
       <c r="P41" s="22"/>
       <c r="Q41" s="22"/>
@@ -1679,26 +1705,26 @@
       <c r="Z41" s="22"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="5" t="s">
-        <v>80</v>
+      <c r="A42" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
       <c r="O42" s="22"/>
       <c r="P42" s="22"/>
       <c r="Q42" s="22"/>
@@ -1713,26 +1739,26 @@
       <c r="Z42" s="22"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="5" t="s">
-        <v>82</v>
+      <c r="A43" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
       <c r="O43" s="22"/>
       <c r="P43" s="22"/>
       <c r="Q43" s="22"/>
@@ -1747,26 +1773,26 @@
       <c r="Z43" s="22"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="5" t="s">
-        <v>84</v>
+      <c r="A44" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
       <c r="O44" s="22"/>
       <c r="P44" s="22"/>
       <c r="Q44" s="22"/>
@@ -1781,26 +1807,26 @@
       <c r="Z44" s="22"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
+      <c r="A45" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
       <c r="O45" s="22"/>
       <c r="P45" s="22"/>
       <c r="Q45" s="22"/>
@@ -1815,26 +1841,26 @@
       <c r="Z45" s="22"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
+      <c r="A46" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
       <c r="O46" s="22"/>
       <c r="P46" s="22"/>
       <c r="Q46" s="22"/>
@@ -1849,26 +1875,26 @@
       <c r="Z46" s="22"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="5" t="s">
-        <v>89</v>
+      <c r="A47" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
       <c r="O47" s="22"/>
       <c r="P47" s="22"/>
       <c r="Q47" s="22"/>
@@ -1883,26 +1909,26 @@
       <c r="Z47" s="22"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
+      <c r="A48" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
       <c r="O48" s="22"/>
       <c r="P48" s="22"/>
       <c r="Q48" s="22"/>
@@ -1917,78 +1943,78 @@
       <c r="Z48" s="22"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="5"/>
-      <c r="U49" s="5"/>
-      <c r="V49" s="5"/>
-      <c r="W49" s="5"/>
-      <c r="X49" s="5"/>
-      <c r="Y49" s="5"/>
-      <c r="Z49" s="5"/>
+      <c r="A49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
     </row>
     <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="5"/>
-      <c r="U50" s="5"/>
-      <c r="V50" s="5"/>
-      <c r="W50" s="5"/>
-      <c r="X50" s="5"/>
-      <c r="Y50" s="5"/>
-      <c r="Z50" s="5"/>
+      <c r="A50" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="A51" s="9"/>
       <c r="B51" s="13"/>
       <c r="C51" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
@@ -2000,51 +2026,375 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
     </row>
     <row r="52">
-      <c r="A52" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C52" s="23" t="s">
+      <c r="A52" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="B52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="4"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>101</v>
-      </c>
+      <c r="A53" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+      <c r="W53" s="4"/>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="4"/>
     </row>
     <row r="54">
-      <c r="A54" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C54" s="23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
+      <c r="A54" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="4"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4"/>
+      <c r="X55" s="4"/>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="4"/>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="4"/>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="4"/>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="4"/>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="4"/>
+      <c r="W59" s="4"/>
+      <c r="X59" s="4"/>
+      <c r="Y59" s="4"/>
+      <c r="Z59" s="4"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
+      <c r="X60" s="4"/>
+      <c r="Y60" s="4"/>
+      <c r="Z60" s="4"/>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="4"/>
+      <c r="X61" s="4"/>
+      <c r="Y61" s="4"/>
+      <c r="Z61" s="4"/>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="4"/>
+      <c r="X62" s="4"/>
+      <c r="Y62" s="4"/>
+      <c r="Z62" s="4"/>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+      <c r="U63" s="4"/>
+      <c r="V63" s="4"/>
+      <c r="W63" s="4"/>
+      <c r="X63" s="4"/>
+      <c r="Y63" s="4"/>
+      <c r="Z63" s="4"/>
+    </row>
     <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
@@ -3003,79 +3353,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added new TCs, functions and test data.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
   <si>
     <t>Variable</t>
   </si>
   <si>
+    <t>Supported Browser Types</t>
+  </si>
+  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -32,36 +35,33 @@
     <t>Data5</t>
   </si>
   <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
     <t>Data6</t>
   </si>
   <si>
+    <t>MicrosoftEdge</t>
+  </si>
+  <si>
     <t>URL_login_login</t>
   </si>
   <si>
     <t>#/login</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>URL_content</t>
   </si>
   <si>
     <t>#/catalog</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>URL_content_allContent</t>
   </si>
   <si>
@@ -342,6 +342,24 @@
   </si>
   <si>
     <t>New Dashboard Created by user "UserWithProfilePicture"</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_GrammerAndCountUnderFolder</t>
+  </si>
+  <si>
+    <t>New Folder</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_FolderInsideFolder</t>
+  </si>
+  <si>
+    <t>New Folder inside folder "Automation_Folder_CatalogOfContent_GrammerAndCountUnderFolder"</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_DashboardInsideFolder</t>
+  </si>
+  <si>
+    <t>New Dashboard inside folder "Automation_Folder_CatalogOfContent_GrammerAndCountUnderFolder"</t>
   </si>
 </sst>
 </file>
@@ -476,6 +494,9 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -489,9 +510,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -579,22 +597,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -606,212 +624,212 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
     </row>
@@ -831,99 +849,99 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
     </row>
@@ -943,54 +961,54 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="7"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="15" t="s">
@@ -999,135 +1017,135 @@
       <c r="B19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
       <c r="O19" s="8"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
       <c r="O20" s="8"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="7"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
       <c r="O22" s="8"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
       <c r="O23" s="8"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
       <c r="O24" s="17"/>
       <c r="P24" s="18"/>
       <c r="Q24" s="18"/>
@@ -1142,26 +1160,26 @@
       <c r="Z24" s="18"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
       <c r="O25" s="17"/>
       <c r="P25" s="18"/>
       <c r="Q25" s="18"/>
@@ -1176,26 +1194,26 @@
       <c r="Z25" s="18"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
       <c r="O26" s="17"/>
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
@@ -1210,26 +1228,26 @@
       <c r="Z26" s="18"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
       <c r="O27" s="17"/>
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
@@ -1244,26 +1262,26 @@
       <c r="Z27" s="18"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
       <c r="O28" s="22"/>
       <c r="P28" s="22"/>
       <c r="Q28" s="22"/>
@@ -1278,26 +1296,26 @@
       <c r="Z28" s="22"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
       <c r="O29" s="22"/>
       <c r="P29" s="22"/>
       <c r="Q29" s="22"/>
@@ -1312,26 +1330,26 @@
       <c r="Z29" s="22"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="22"/>
@@ -1346,26 +1364,26 @@
       <c r="Z30" s="22"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
       <c r="O31" s="22"/>
       <c r="P31" s="22"/>
       <c r="Q31" s="22"/>
@@ -1395,30 +1413,30 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
       <c r="O33" s="22"/>
       <c r="P33" s="22"/>
       <c r="Q33" s="22"/>
@@ -1433,26 +1451,26 @@
       <c r="Z33" s="22"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
       <c r="O34" s="22"/>
       <c r="P34" s="22"/>
       <c r="Q34" s="22"/>
@@ -1473,20 +1491,20 @@
       <c r="B35" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
       <c r="O35" s="22"/>
       <c r="P35" s="22"/>
       <c r="Q35" s="22"/>
@@ -1501,26 +1519,26 @@
       <c r="Z35" s="22"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
       <c r="O36" s="22"/>
       <c r="P36" s="22"/>
       <c r="Q36" s="22"/>
@@ -1535,26 +1553,26 @@
       <c r="Z36" s="22"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
       <c r="O37" s="22"/>
       <c r="P37" s="22"/>
       <c r="Q37" s="22"/>
@@ -1569,26 +1587,26 @@
       <c r="Z37" s="22"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
       <c r="O38" s="22"/>
       <c r="P38" s="22"/>
       <c r="Q38" s="22"/>
@@ -1603,26 +1621,26 @@
       <c r="Z38" s="22"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
       <c r="O39" s="22"/>
       <c r="P39" s="22"/>
       <c r="Q39" s="22"/>
@@ -1637,26 +1655,26 @@
       <c r="Z39" s="22"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
       <c r="O40" s="22"/>
       <c r="P40" s="22"/>
       <c r="Q40" s="22"/>
@@ -1671,26 +1689,26 @@
       <c r="Z40" s="22"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
       <c r="O41" s="22"/>
       <c r="P41" s="22"/>
       <c r="Q41" s="22"/>
@@ -1705,26 +1723,26 @@
       <c r="Z41" s="22"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
       <c r="O42" s="22"/>
       <c r="P42" s="22"/>
       <c r="Q42" s="22"/>
@@ -1739,26 +1757,26 @@
       <c r="Z42" s="22"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
       <c r="O43" s="22"/>
       <c r="P43" s="22"/>
       <c r="Q43" s="22"/>
@@ -1773,26 +1791,26 @@
       <c r="Z43" s="22"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
       <c r="O44" s="22"/>
       <c r="P44" s="22"/>
       <c r="Q44" s="22"/>
@@ -1807,26 +1825,26 @@
       <c r="Z44" s="22"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
       <c r="O45" s="22"/>
       <c r="P45" s="22"/>
       <c r="Q45" s="22"/>
@@ -1841,26 +1859,26 @@
       <c r="Z45" s="22"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
       <c r="O46" s="22"/>
       <c r="P46" s="22"/>
       <c r="Q46" s="22"/>
@@ -1875,26 +1893,26 @@
       <c r="Z46" s="22"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
       <c r="O47" s="22"/>
       <c r="P47" s="22"/>
       <c r="Q47" s="22"/>
@@ -1909,26 +1927,26 @@
       <c r="Z47" s="22"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
       <c r="O48" s="22"/>
       <c r="P48" s="22"/>
       <c r="Q48" s="22"/>
@@ -1943,72 +1961,72 @@
       <c r="Z48" s="22"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
-      <c r="W49" s="4"/>
-      <c r="X49" s="4"/>
-      <c r="Y49" s="4"/>
-      <c r="Z49" s="4"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="5"/>
     </row>
     <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
-      <c r="S50" s="4"/>
-      <c r="T50" s="4"/>
-      <c r="U50" s="4"/>
-      <c r="V50" s="4"/>
-      <c r="W50" s="4"/>
-      <c r="X50" s="4"/>
-      <c r="Y50" s="4"/>
-      <c r="Z50" s="4"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5"/>
+      <c r="W50" s="5"/>
+      <c r="X50" s="5"/>
+      <c r="Y50" s="5"/>
+      <c r="Z50" s="5"/>
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="A51" s="9"/>
@@ -2026,110 +2044,110 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
-      <c r="Q52" s="4"/>
-      <c r="R52" s="4"/>
-      <c r="S52" s="4"/>
-      <c r="T52" s="4"/>
-      <c r="U52" s="4"/>
-      <c r="V52" s="4"/>
-      <c r="W52" s="4"/>
-      <c r="X52" s="4"/>
-      <c r="Y52" s="4"/>
-      <c r="Z52" s="4"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
+      <c r="V52" s="5"/>
+      <c r="W52" s="5"/>
+      <c r="X52" s="5"/>
+      <c r="Y52" s="5"/>
+      <c r="Z52" s="5"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
-      <c r="Q53" s="4"/>
-      <c r="R53" s="4"/>
-      <c r="S53" s="4"/>
-      <c r="T53" s="4"/>
-      <c r="U53" s="4"/>
-      <c r="V53" s="4"/>
-      <c r="W53" s="4"/>
-      <c r="X53" s="4"/>
-      <c r="Y53" s="4"/>
-      <c r="Z53" s="4"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
-      <c r="Q54" s="4"/>
-      <c r="R54" s="4"/>
-      <c r="S54" s="4"/>
-      <c r="T54" s="4"/>
-      <c r="U54" s="4"/>
-      <c r="V54" s="4"/>
-      <c r="W54" s="4"/>
-      <c r="X54" s="4"/>
-      <c r="Y54" s="4"/>
-      <c r="Z54" s="4"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="23" t="s">
@@ -2138,32 +2156,32 @@
       <c r="B55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
-      <c r="V55" s="4"/>
-      <c r="W55" s="4"/>
-      <c r="X55" s="4"/>
-      <c r="Y55" s="4"/>
-      <c r="Z55" s="4"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="5"/>
+      <c r="T55" s="5"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="5"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="23" t="s">
@@ -2172,228 +2190,246 @@
       <c r="B56" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4"/>
-      <c r="Q56" s="4"/>
-      <c r="R56" s="4"/>
-      <c r="S56" s="4"/>
-      <c r="T56" s="4"/>
-      <c r="U56" s="4"/>
-      <c r="V56" s="4"/>
-      <c r="W56" s="4"/>
-      <c r="X56" s="4"/>
-      <c r="Y56" s="4"/>
-      <c r="Z56" s="4"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="5"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
-      <c r="Q57" s="4"/>
-      <c r="R57" s="4"/>
-      <c r="S57" s="4"/>
-      <c r="T57" s="4"/>
-      <c r="U57" s="4"/>
-      <c r="V57" s="4"/>
-      <c r="W57" s="4"/>
-      <c r="X57" s="4"/>
-      <c r="Y57" s="4"/>
-      <c r="Z57" s="4"/>
+      <c r="A57" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="5"/>
+      <c r="T57" s="5"/>
+      <c r="U57" s="5"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="5"/>
+      <c r="Y57" s="5"/>
+      <c r="Z57" s="5"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
-      <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="4"/>
-      <c r="V58" s="4"/>
-      <c r="W58" s="4"/>
-      <c r="X58" s="4"/>
-      <c r="Y58" s="4"/>
-      <c r="Z58" s="4"/>
+      <c r="A58" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5"/>
+      <c r="T58" s="5"/>
+      <c r="U58" s="5"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="5"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
-      <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
-      <c r="U59" s="4"/>
-      <c r="V59" s="4"/>
-      <c r="W59" s="4"/>
-      <c r="X59" s="4"/>
-      <c r="Y59" s="4"/>
-      <c r="Z59" s="4"/>
+      <c r="A59" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5"/>
+      <c r="V59" s="5"/>
+      <c r="W59" s="5"/>
+      <c r="X59" s="5"/>
+      <c r="Y59" s="5"/>
+      <c r="Z59" s="5"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
-      <c r="S60" s="4"/>
-      <c r="T60" s="4"/>
-      <c r="U60" s="4"/>
-      <c r="V60" s="4"/>
-      <c r="W60" s="4"/>
-      <c r="X60" s="4"/>
-      <c r="Y60" s="4"/>
-      <c r="Z60" s="4"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5"/>
+      <c r="S60" s="5"/>
+      <c r="T60" s="5"/>
+      <c r="U60" s="5"/>
+      <c r="V60" s="5"/>
+      <c r="W60" s="5"/>
+      <c r="X60" s="5"/>
+      <c r="Y60" s="5"/>
+      <c r="Z60" s="5"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
-      <c r="U61" s="4"/>
-      <c r="V61" s="4"/>
-      <c r="W61" s="4"/>
-      <c r="X61" s="4"/>
-      <c r="Y61" s="4"/>
-      <c r="Z61" s="4"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="5"/>
+      <c r="U61" s="5"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="5"/>
+      <c r="Z61" s="5"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
-      <c r="Q62" s="4"/>
-      <c r="R62" s="4"/>
-      <c r="S62" s="4"/>
-      <c r="T62" s="4"/>
-      <c r="U62" s="4"/>
-      <c r="V62" s="4"/>
-      <c r="W62" s="4"/>
-      <c r="X62" s="4"/>
-      <c r="Y62" s="4"/>
-      <c r="Z62" s="4"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="5"/>
+      <c r="T62" s="5"/>
+      <c r="U62" s="5"/>
+      <c r="V62" s="5"/>
+      <c r="W62" s="5"/>
+      <c r="X62" s="5"/>
+      <c r="Y62" s="5"/>
+      <c r="Z62" s="5"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-      <c r="S63" s="4"/>
-      <c r="T63" s="4"/>
-      <c r="U63" s="4"/>
-      <c r="V63" s="4"/>
-      <c r="W63" s="4"/>
-      <c r="X63" s="4"/>
-      <c r="Y63" s="4"/>
-      <c r="Z63" s="4"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="5"/>
+      <c r="T63" s="5"/>
+      <c r="U63" s="5"/>
+      <c r="V63" s="5"/>
+      <c r="W63" s="5"/>
+      <c r="X63" s="5"/>
+      <c r="Y63" s="5"/>
+      <c r="Z63" s="5"/>
     </row>
     <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
@@ -3353,79 +3389,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Finalizing TCs and functions. Re-factoring and fixing test cases issues. Added new test data.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="135">
   <si>
     <t>Variable</t>
   </si>
@@ -44,12 +44,12 @@
     <t>MicrosoftInternetExplorer</t>
   </si>
   <si>
+    <t>MicrosoftEdge</t>
+  </si>
+  <si>
     <t>Data6</t>
   </si>
   <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>URL_login_login</t>
   </si>
   <si>
@@ -360,6 +360,63 @@
   </si>
   <si>
     <t>New Dashboard inside folder "Automation_Folder_CatalogOfContent_GrammerAndCountUnderFolder"</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_Sort</t>
+  </si>
+  <si>
+    <t>New folder - Shared edit with admin</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_SortB</t>
+  </si>
+  <si>
+    <t>New Dashbord Inside above folder - First one to be created by Analyzer</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_SortA</t>
+  </si>
+  <si>
+    <t>New Dashbord Inside above folder - Second one to be created by Admin</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_SortC</t>
+  </si>
+  <si>
+    <t>New Dashbord Inside above folder - Third one to be created by Analyzer</t>
+  </si>
+  <si>
+    <t>SortDashboardByOwner</t>
+  </si>
+  <si>
+    <t>SortDashboardByLastModified</t>
+  </si>
+  <si>
+    <t>SortDashboardByName</t>
+  </si>
+  <si>
+    <t>FoldersIsOneAndDashboardsIsOne</t>
+  </si>
+  <si>
+    <t>1 Folder and 1 Dashboard</t>
+  </si>
+  <si>
+    <t>FoldersIsZeroAndDashboardsIsTwo</t>
+  </si>
+  <si>
+    <t>0 Folders and 2 Dashboards</t>
+  </si>
+  <si>
+    <t>Automation_Folder_CatalogOfContent_GrammerAndCountUnderFolder_Number2</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_Dashboard1</t>
+  </si>
+  <si>
+    <t>New Dashboard under above folder</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CatalogOfContent_Dashboard2</t>
   </si>
 </sst>
 </file>
@@ -612,7 +669,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2319,38 +2376,33 @@
       <c r="Y59" s="5"/>
       <c r="Z59" s="5"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="5"/>
-      <c r="P60" s="5"/>
-      <c r="Q60" s="5"/>
-      <c r="R60" s="5"/>
-      <c r="S60" s="5"/>
-      <c r="T60" s="5"/>
-      <c r="U60" s="5"/>
-      <c r="V60" s="5"/>
-      <c r="W60" s="5"/>
-      <c r="X60" s="5"/>
-      <c r="Y60" s="5"/>
-      <c r="Z60" s="5"/>
+    <row r="60" ht="13.5" customHeight="1">
+      <c r="A60" s="9"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
+      <c r="A61" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
@@ -2376,9 +2428,15 @@
       <c r="Z61" s="5"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
+      <c r="A62" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -2404,9 +2462,15 @@
       <c r="Z62" s="5"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
+      <c r="A63" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
@@ -2431,28 +2495,656 @@
       <c r="Y63" s="5"/>
       <c r="Z63" s="5"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="A64" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="5"/>
+      <c r="P64" s="5"/>
+      <c r="Q64" s="5"/>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5"/>
+      <c r="T64" s="5"/>
+      <c r="U64" s="5"/>
+      <c r="V64" s="5"/>
+      <c r="W64" s="5"/>
+      <c r="X64" s="5"/>
+      <c r="Y64" s="5"/>
+      <c r="Z64" s="5"/>
+    </row>
+    <row r="65" ht="13.5" customHeight="1">
+      <c r="A65" s="9"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+    </row>
+    <row r="66" ht="15.75" customHeight="1">
+      <c r="A66" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="5"/>
+      <c r="Q66" s="5"/>
+      <c r="R66" s="5"/>
+      <c r="S66" s="5"/>
+      <c r="T66" s="5"/>
+      <c r="U66" s="5"/>
+      <c r="V66" s="5"/>
+      <c r="W66" s="5"/>
+      <c r="X66" s="5"/>
+      <c r="Y66" s="5"/>
+      <c r="Z66" s="5"/>
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="A67" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="5"/>
+      <c r="R67" s="5"/>
+      <c r="S67" s="5"/>
+      <c r="T67" s="5"/>
+      <c r="U67" s="5"/>
+      <c r="V67" s="5"/>
+      <c r="W67" s="5"/>
+      <c r="X67" s="5"/>
+      <c r="Y67" s="5"/>
+      <c r="Z67" s="5"/>
+    </row>
+    <row r="68" ht="15.75" customHeight="1">
+      <c r="A68" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="5"/>
+      <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
+      <c r="T68" s="5"/>
+      <c r="U68" s="5"/>
+      <c r="V68" s="5"/>
+      <c r="W68" s="5"/>
+      <c r="X68" s="5"/>
+      <c r="Y68" s="5"/>
+      <c r="Z68" s="5"/>
+    </row>
+    <row r="69" ht="13.5" customHeight="1">
+      <c r="A69" s="9"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="7"/>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="A70" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="5"/>
+      <c r="P70" s="5"/>
+      <c r="Q70" s="5"/>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
+      <c r="U70" s="5"/>
+      <c r="V70" s="5"/>
+      <c r="W70" s="5"/>
+      <c r="X70" s="5"/>
+      <c r="Y70" s="5"/>
+      <c r="Z70" s="5"/>
+    </row>
+    <row r="71" ht="15.75" customHeight="1">
+      <c r="A71" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+      <c r="O71" s="5"/>
+      <c r="P71" s="5"/>
+      <c r="Q71" s="5"/>
+      <c r="R71" s="5"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="5"/>
+      <c r="U71" s="5"/>
+      <c r="V71" s="5"/>
+      <c r="W71" s="5"/>
+      <c r="X71" s="5"/>
+      <c r="Y71" s="5"/>
+      <c r="Z71" s="5"/>
+    </row>
+    <row r="72" ht="15.75" customHeight="1">
+      <c r="A72" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
+      <c r="N72" s="5"/>
+      <c r="O72" s="5"/>
+      <c r="P72" s="5"/>
+      <c r="Q72" s="5"/>
+      <c r="R72" s="5"/>
+      <c r="S72" s="5"/>
+      <c r="T72" s="5"/>
+      <c r="U72" s="5"/>
+      <c r="V72" s="5"/>
+      <c r="W72" s="5"/>
+      <c r="X72" s="5"/>
+      <c r="Y72" s="5"/>
+      <c r="Z72" s="5"/>
+    </row>
+    <row r="73" ht="15.75" customHeight="1">
+      <c r="A73" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="5"/>
+      <c r="O73" s="5"/>
+      <c r="P73" s="5"/>
+      <c r="Q73" s="5"/>
+      <c r="R73" s="5"/>
+      <c r="S73" s="5"/>
+      <c r="T73" s="5"/>
+      <c r="U73" s="5"/>
+      <c r="V73" s="5"/>
+      <c r="W73" s="5"/>
+      <c r="X73" s="5"/>
+      <c r="Y73" s="5"/>
+      <c r="Z73" s="5"/>
+    </row>
+    <row r="74" ht="15.75" customHeight="1">
+      <c r="A74" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="5"/>
+      <c r="P74" s="5"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5"/>
+      <c r="S74" s="5"/>
+      <c r="T74" s="5"/>
+      <c r="U74" s="5"/>
+      <c r="V74" s="5"/>
+      <c r="W74" s="5"/>
+      <c r="X74" s="5"/>
+      <c r="Y74" s="5"/>
+      <c r="Z74" s="5"/>
+    </row>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5"/>
+      <c r="Q75" s="5"/>
+      <c r="R75" s="5"/>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
+      <c r="U75" s="5"/>
+      <c r="V75" s="5"/>
+      <c r="W75" s="5"/>
+      <c r="X75" s="5"/>
+      <c r="Y75" s="5"/>
+      <c r="Z75" s="5"/>
+    </row>
+    <row r="76" ht="15.75" customHeight="1">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
+      <c r="U76" s="5"/>
+      <c r="V76" s="5"/>
+      <c r="W76" s="5"/>
+      <c r="X76" s="5"/>
+      <c r="Y76" s="5"/>
+      <c r="Z76" s="5"/>
+    </row>
+    <row r="77" ht="15.75" customHeight="1">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
+      <c r="O77" s="5"/>
+      <c r="P77" s="5"/>
+      <c r="Q77" s="5"/>
+      <c r="R77" s="5"/>
+      <c r="S77" s="5"/>
+      <c r="T77" s="5"/>
+      <c r="U77" s="5"/>
+      <c r="V77" s="5"/>
+      <c r="W77" s="5"/>
+      <c r="X77" s="5"/>
+      <c r="Y77" s="5"/>
+      <c r="Z77" s="5"/>
+    </row>
+    <row r="78" ht="15.75" customHeight="1">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+      <c r="O78" s="5"/>
+      <c r="P78" s="5"/>
+      <c r="Q78" s="5"/>
+      <c r="R78" s="5"/>
+      <c r="S78" s="5"/>
+      <c r="T78" s="5"/>
+      <c r="U78" s="5"/>
+      <c r="V78" s="5"/>
+      <c r="W78" s="5"/>
+      <c r="X78" s="5"/>
+      <c r="Y78" s="5"/>
+      <c r="Z78" s="5"/>
+    </row>
+    <row r="79" ht="15.75" customHeight="1">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+      <c r="P79" s="5"/>
+      <c r="Q79" s="5"/>
+      <c r="R79" s="5"/>
+      <c r="S79" s="5"/>
+      <c r="T79" s="5"/>
+      <c r="U79" s="5"/>
+      <c r="V79" s="5"/>
+      <c r="W79" s="5"/>
+      <c r="X79" s="5"/>
+      <c r="Y79" s="5"/>
+      <c r="Z79" s="5"/>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="5"/>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="5"/>
+      <c r="R80" s="5"/>
+      <c r="S80" s="5"/>
+      <c r="T80" s="5"/>
+      <c r="U80" s="5"/>
+      <c r="V80" s="5"/>
+      <c r="W80" s="5"/>
+      <c r="X80" s="5"/>
+      <c r="Y80" s="5"/>
+      <c r="Z80" s="5"/>
+    </row>
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5"/>
+      <c r="O81" s="5"/>
+      <c r="P81" s="5"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="5"/>
+      <c r="S81" s="5"/>
+      <c r="T81" s="5"/>
+      <c r="U81" s="5"/>
+      <c r="V81" s="5"/>
+      <c r="W81" s="5"/>
+      <c r="X81" s="5"/>
+      <c r="Y81" s="5"/>
+      <c r="Z81" s="5"/>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5"/>
+      <c r="O82" s="5"/>
+      <c r="P82" s="5"/>
+      <c r="Q82" s="5"/>
+      <c r="R82" s="5"/>
+      <c r="S82" s="5"/>
+      <c r="T82" s="5"/>
+      <c r="U82" s="5"/>
+      <c r="V82" s="5"/>
+      <c r="W82" s="5"/>
+      <c r="X82" s="5"/>
+      <c r="Y82" s="5"/>
+      <c r="Z82" s="5"/>
+    </row>
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="5"/>
+      <c r="P83" s="5"/>
+      <c r="Q83" s="5"/>
+      <c r="R83" s="5"/>
+      <c r="S83" s="5"/>
+      <c r="T83" s="5"/>
+      <c r="U83" s="5"/>
+      <c r="V83" s="5"/>
+      <c r="W83" s="5"/>
+      <c r="X83" s="5"/>
+      <c r="Y83" s="5"/>
+      <c r="Z83" s="5"/>
+    </row>
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="5"/>
+      <c r="O84" s="5"/>
+      <c r="P84" s="5"/>
+      <c r="Q84" s="5"/>
+      <c r="R84" s="5"/>
+      <c r="S84" s="5"/>
+      <c r="T84" s="5"/>
+      <c r="U84" s="5"/>
+      <c r="V84" s="5"/>
+      <c r="W84" s="5"/>
+      <c r="X84" s="5"/>
+      <c r="Y84" s="5"/>
+      <c r="Z84" s="5"/>
+    </row>
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5"/>
+      <c r="O85" s="5"/>
+      <c r="P85" s="5"/>
+      <c r="Q85" s="5"/>
+      <c r="R85" s="5"/>
+      <c r="S85" s="5"/>
+      <c r="T85" s="5"/>
+      <c r="U85" s="5"/>
+      <c r="V85" s="5"/>
+      <c r="W85" s="5"/>
+      <c r="X85" s="5"/>
+      <c r="Y85" s="5"/>
+      <c r="Z85" s="5"/>
+    </row>
     <row r="86" ht="15.75" customHeight="1"/>
     <row r="87" ht="15.75" customHeight="1"/>
     <row r="88" ht="15.75" customHeight="1"/>
@@ -3450,7 +4142,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>

</xml_diff>

<commit_message>
Updating tenant name from demo to "content test"
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/catalogOfContent_newUI/TestData.xlsx
@@ -12,14 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="137">
+  <si>
+    <t>Supported Browser Types</t>
+  </si>
   <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -35,9 +35,18 @@
     <t>Data5</t>
   </si>
   <si>
+    <t>Data6</t>
+  </si>
+  <si>
+    <t>URL_login_login</t>
+  </si>
+  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
+    <t>#/login</t>
+  </si>
+  <si>
     <t>GoogleChrome</t>
   </si>
   <si>
@@ -47,15 +56,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Data6</t>
-  </si>
-  <si>
-    <t>URL_login_login</t>
-  </si>
-  <si>
-    <t>#/login</t>
-  </si>
-  <si>
     <t>URL_content</t>
   </si>
   <si>
@@ -113,7 +113,7 @@
     <t>Tenant</t>
   </si>
   <si>
-    <t>Demo</t>
+    <t>content_test</t>
   </si>
   <si>
     <t>Username</t>
@@ -140,7 +140,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Automation_Analyzer1</t>
+    <t>Automation_Analyzer11</t>
   </si>
   <si>
     <t>Comments</t>
@@ -245,13 +245,19 @@
     <t>Automation_Folder_CatalogOfContent2.1</t>
   </si>
   <si>
+    <t>new folder inside Automation_Folder_CatalogOfContent1.1</t>
+  </si>
+  <si>
     <t>Automation_Folder_CatalogOfContent3.1</t>
   </si>
   <si>
+    <t>new folder inside Automation_Folder_CatalogOfContent2.1</t>
+  </si>
+  <si>
     <t>Automation_Folder_CatalogOfContent_InsideNestedFolder</t>
   </si>
   <si>
-    <t>New Folder inside Automation_Folder_CatalogOfContent3</t>
+    <t>New Folder inside Automation_Folder_CatalogOfContent3.1</t>
   </si>
   <si>
     <t>Automation_Folder_CatalogOfContent_Arabic</t>
@@ -365,7 +371,7 @@
     <t>Automation_Dashboard_CatalogOfContent_Sort</t>
   </si>
   <si>
-    <t>New folder - Shared edit with admin</t>
+    <t>New Folder - Shared edit with admin</t>
   </si>
   <si>
     <t>Automation_Dashboard_CatalogOfContent_SortB</t>
@@ -548,11 +554,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -645,47 +651,48 @@
     <col customWidth="1" min="4" max="4" width="21.71"/>
     <col customWidth="1" min="5" max="5" width="27.43"/>
     <col customWidth="1" min="6" max="6" width="16.86"/>
-    <col customWidth="1" min="7" max="15" width="8.57"/>
+    <col customWidth="1" min="7" max="7" width="22.14"/>
+    <col customWidth="1" min="8" max="15" width="8.57"/>
     <col customWidth="1" min="16" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -1651,7 +1658,7 @@
         <v>76</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1682,10 +1689,10 @@
         <v>54</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1713,13 +1720,13 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -1747,10 +1754,10 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>51</v>
@@ -1781,10 +1788,10 @@
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="A42" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>51</v>
@@ -1815,10 +1822,10 @@
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>51</v>
@@ -1849,10 +1856,10 @@
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="A44" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>51</v>
@@ -1883,10 +1890,10 @@
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>51</v>
@@ -1917,13 +1924,13 @@
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="A46" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -1951,13 +1958,13 @@
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -1985,13 +1992,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -2019,13 +2026,13 @@
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -2053,13 +2060,13 @@
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -2106,13 +2113,13 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -2140,13 +2147,13 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -2174,13 +2181,13 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
@@ -2208,13 +2215,13 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
@@ -2242,13 +2249,13 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
@@ -2276,13 +2283,13 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
@@ -2310,13 +2317,13 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
@@ -2344,13 +2351,13 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="23" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
@@ -2395,13 +2402,13 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -2429,13 +2436,13 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
@@ -2463,13 +2470,13 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
@@ -2497,13 +2504,13 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
@@ -2548,16 +2555,16 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
@@ -2584,16 +2591,16 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
@@ -2620,16 +2627,16 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B68" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>118</v>
-      </c>
       <c r="D68" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
@@ -2673,10 +2680,10 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -2705,10 +2712,10 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -2737,13 +2744,13 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -2771,13 +2778,13 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
@@ -2805,13 +2812,13 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
@@ -4081,79 +4088,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>